<commit_message>
initial changes on merging workflows for kp and hts
</commit_message>
<xml_diff>
--- a/config/default/forms/contact/health_center-create.xlsx
+++ b/config/default/forms/contact/health_center-create.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="996" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="994" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="378">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -612,6 +612,7 @@
         <color rgb="FF000000"/>
         <rFont val="FreeSans"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">बाहरी </t>
     </r>
@@ -639,6 +640,7 @@
         <color rgb="FF000000"/>
         <rFont val="FreeSans"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">बाहिरि </t>
     </r>
@@ -711,6 +713,7 @@
         <color rgb="FF000000"/>
         <rFont val="FreeSans"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">क्या आप इस स्थान को प्राथमिक कॉंटॅक्ट का नाम देना चाहेंगे</t>
     </r>
@@ -738,6 +741,7 @@
         <color rgb="FF000000"/>
         <rFont val="FreeSans"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">के तपाइ यस स्थानकाे प्राथमिक सम्पर्क नाम दिन चाहानु हुन्छ</t>
     </r>
@@ -1026,6 +1030,30 @@
     <t xml:space="preserve">Staff médical</t>
   </si>
   <si>
+    <t xml:space="preserve">kp_case_manager</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KP Case manager</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kp_peer_educator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KP Peer educator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hts_provider</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HTS provider</t>
+  </si>
+  <si>
+    <t xml:space="preserve">clinician</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clinician</t>
+  </si>
+  <si>
     <t xml:space="preserve">other</t>
   </si>
   <si>
@@ -1058,6 +1086,7 @@
         <sz val="11"/>
         <rFont val="FreeSans"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">नहीं</t>
     </r>
@@ -1075,6 +1104,7 @@
         <sz val="11"/>
         <rFont val="FreeSans"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">मैं इसे मैन्युअल रूप से नाम देना चाहता हूं</t>
     </r>
@@ -1091,6 +1121,7 @@
         <sz val="11"/>
         <rFont val="FreeSans"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">होइन</t>
     </r>
@@ -1108,6 +1139,7 @@
         <sz val="11"/>
         <rFont val="FreeSans"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">म आफैँ नाम दिन चाहन्छु</t>
     </r>
@@ -1193,6 +1225,7 @@
         <sz val="11"/>
         <rFont val="FreeSans"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">का ज़िला</t>
     </r>
@@ -1218,6 +1251,7 @@
         <sz val="11"/>
         <rFont val="FreeSans"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">को जिल्ला </t>
     </r>
@@ -1243,6 +1277,7 @@
         <sz val="11"/>
         <rFont val="FreeSans"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">का स्वास्थ्य केंद्र</t>
     </r>
@@ -1268,6 +1303,7 @@
         <sz val="11"/>
         <rFont val="FreeSans"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">को स्वास्थ्य केन्द्र</t>
     </r>
@@ -1293,6 +1329,7 @@
         <sz val="11"/>
         <rFont val="FreeSans"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">का क्षेत्र</t>
     </r>
@@ -1320,6 +1357,7 @@
         <color rgb="FF000000"/>
         <rFont val="FreeSans"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">को क्षेत्र</t>
     </r>
@@ -1402,6 +1440,7 @@
       <color rgb="FF000000"/>
       <name val="FreeSans"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1420,6 +1459,7 @@
       <sz val="11"/>
       <name val="FreeSans"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="12">
@@ -1778,31 +1818,29 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.1887755102041"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.4897959183673"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="49.4948979591837"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="34.6479591836735"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.4387755102041"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="38.6071428571429"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="32.3979591836735"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.45918367346939"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.45918367346939"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="53.2755102040816"/>
-    <col collapsed="false" hidden="false" max="13" min="12" style="0" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="26.1887755102041"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="47.8775510204082"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="71.2755102040816"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="34.6479591836735"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="37.5255102040816"/>
-    <col collapsed="false" hidden="false" max="23" min="20" style="0" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="7.91836734693878"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="9"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="37.0765306122449"/>
-    <col collapsed="false" hidden="false" max="36" min="27" style="0" width="7.91836734693878"/>
-    <col collapsed="false" hidden="false" max="38" min="37" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="44" min="39" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.7091836734694"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.1071428571429"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="53.0051020408163"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="37.0765306122449"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="30.5102040816327"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="41.3979591836735"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="34.6479591836735"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.4489795918367"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="57.1479591836735"/>
+    <col collapsed="false" hidden="false" max="13" min="12" style="0" width="11.7908163265306"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="28.0765306122449"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="51.2959183673469"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="76.4948979591837"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="10.4387755102041"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="37.0765306122449"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="40.3163265306123"/>
+    <col collapsed="false" hidden="false" max="23" min="20" style="0" width="14.9387755102041"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="8.45918367346939"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="9.54081632653061"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="39.7755102040816"/>
+    <col collapsed="false" hidden="false" max="36" min="27" style="0" width="8.45918367346939"/>
+    <col collapsed="false" hidden="false" max="38" min="37" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="44" min="39" style="0" width="19.0765306122449"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6021,23 +6059,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z65536"/>
+  <dimension ref="A1:Z27"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.8673469387755"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.969387755102"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="37.5255102040816"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.2602040816327"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="25.5561224489796"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="7.91836734693878"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="14.7602040816327"/>
-    <col collapsed="false" hidden="false" max="13" min="10" style="0" width="7.91836734693878"/>
-    <col collapsed="false" hidden="false" max="26" min="14" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.3979591836735"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.1275510204082"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="40.3163265306123"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="30.3265306122449"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="27.3571428571429"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.45918367346939"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="13" min="10" style="0" width="8.45918367346939"/>
+    <col collapsed="false" hidden="false" max="26" min="14" style="0" width="16.7397959183673"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6614,22 +6652,12 @@
       <c r="C14" s="35" t="s">
         <v>309</v>
       </c>
-      <c r="D14" s="28" t="s">
-        <v>310</v>
-      </c>
-      <c r="E14" s="33" t="s">
-        <v>311</v>
-      </c>
-      <c r="F14" s="29" t="s">
-        <v>312</v>
-      </c>
-      <c r="G14" s="30" t="s">
-        <v>310</v>
-      </c>
+      <c r="D14" s="28"/>
+      <c r="E14" s="33"/>
+      <c r="F14" s="29"/>
+      <c r="G14" s="30"/>
       <c r="H14" s="31"/>
-      <c r="I14" s="20" t="s">
-        <v>313</v>
-      </c>
+      <c r="I14" s="20"/>
       <c r="J14" s="8"/>
       <c r="K14" s="8"/>
       <c r="L14" s="8"/>
@@ -6649,31 +6677,21 @@
       <c r="Z14" s="8"/>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="27" t="s">
-        <v>314</v>
-      </c>
-      <c r="B15" s="27" t="s">
-        <v>219</v>
-      </c>
-      <c r="C15" s="27" t="s">
-        <v>228</v>
-      </c>
-      <c r="D15" s="28" t="s">
-        <v>229</v>
-      </c>
-      <c r="E15" s="12" t="s">
-        <v>230</v>
-      </c>
-      <c r="F15" s="29" t="s">
-        <v>231</v>
-      </c>
-      <c r="G15" s="30" t="s">
-        <v>315</v>
-      </c>
+      <c r="A15" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="B15" s="34" t="s">
+        <v>310</v>
+      </c>
+      <c r="C15" s="35" t="s">
+        <v>311</v>
+      </c>
+      <c r="D15" s="28"/>
+      <c r="E15" s="33"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="30"/>
       <c r="H15" s="31"/>
-      <c r="I15" s="20" t="s">
-        <v>233</v>
-      </c>
+      <c r="I15" s="20"/>
       <c r="J15" s="8"/>
       <c r="K15" s="8"/>
       <c r="L15" s="8"/>
@@ -6693,31 +6711,21 @@
       <c r="Z15" s="8"/>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="27" t="s">
-        <v>314</v>
-      </c>
-      <c r="B16" s="27" t="s">
-        <v>234</v>
-      </c>
-      <c r="C16" s="27" t="s">
-        <v>316</v>
-      </c>
-      <c r="D16" s="28" t="s">
-        <v>317</v>
-      </c>
-      <c r="E16" s="33" t="s">
-        <v>318</v>
-      </c>
-      <c r="F16" s="29" t="s">
-        <v>319</v>
-      </c>
-      <c r="G16" s="30" t="s">
-        <v>320</v>
-      </c>
+      <c r="A16" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="B16" s="34" t="s">
+        <v>312</v>
+      </c>
+      <c r="C16" s="35" t="s">
+        <v>313</v>
+      </c>
+      <c r="D16" s="28"/>
+      <c r="E16" s="33"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="30"/>
       <c r="H16" s="31"/>
-      <c r="I16" s="20" t="s">
-        <v>321</v>
-      </c>
+      <c r="I16" s="20"/>
       <c r="J16" s="8"/>
       <c r="K16" s="8"/>
       <c r="L16" s="8"/>
@@ -6738,30 +6746,20 @@
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="8" t="s">
-        <v>73</v>
+        <v>280</v>
       </c>
       <c r="B17" s="34" t="s">
-        <v>322</v>
+        <v>314</v>
       </c>
       <c r="C17" s="35" t="s">
-        <v>323</v>
-      </c>
-      <c r="D17" s="28" t="s">
-        <v>324</v>
-      </c>
-      <c r="E17" s="33" t="s">
-        <v>325</v>
-      </c>
-      <c r="F17" s="29" t="s">
-        <v>326</v>
-      </c>
-      <c r="G17" s="30" t="s">
-        <v>327</v>
-      </c>
+        <v>315</v>
+      </c>
+      <c r="D17" s="28"/>
+      <c r="E17" s="33"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="30"/>
       <c r="H17" s="31"/>
-      <c r="I17" s="20" t="s">
-        <v>328</v>
-      </c>
+      <c r="I17" s="20"/>
       <c r="J17" s="8"/>
       <c r="K17" s="8"/>
       <c r="L17" s="8"/>
@@ -6782,29 +6780,29 @@
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="8" t="s">
-        <v>73</v>
+        <v>280</v>
       </c>
       <c r="B18" s="34" t="s">
-        <v>329</v>
+        <v>316</v>
       </c>
       <c r="C18" s="35" t="s">
-        <v>330</v>
+        <v>317</v>
       </c>
       <c r="D18" s="28" t="s">
-        <v>331</v>
+        <v>318</v>
       </c>
       <c r="E18" s="33" t="s">
-        <v>332</v>
+        <v>319</v>
       </c>
       <c r="F18" s="29" t="s">
-        <v>333</v>
+        <v>320</v>
       </c>
       <c r="G18" s="30" t="s">
-        <v>334</v>
+        <v>318</v>
       </c>
       <c r="H18" s="31"/>
       <c r="I18" s="20" t="s">
-        <v>335</v>
+        <v>321</v>
       </c>
       <c r="J18" s="8"/>
       <c r="K18" s="8"/>
@@ -6825,30 +6823,30 @@
       <c r="Z18" s="8"/>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="B19" s="34" t="s">
-        <v>336</v>
-      </c>
-      <c r="C19" s="35" t="s">
-        <v>337</v>
+      <c r="A19" s="27" t="s">
+        <v>322</v>
+      </c>
+      <c r="B19" s="27" t="s">
+        <v>219</v>
+      </c>
+      <c r="C19" s="27" t="s">
+        <v>228</v>
       </c>
       <c r="D19" s="28" t="s">
-        <v>338</v>
-      </c>
-      <c r="E19" s="33" t="s">
-        <v>339</v>
+        <v>229</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>230</v>
       </c>
       <c r="F19" s="29" t="s">
-        <v>340</v>
+        <v>231</v>
       </c>
       <c r="G19" s="30" t="s">
-        <v>338</v>
+        <v>323</v>
       </c>
       <c r="H19" s="31"/>
       <c r="I19" s="20" t="s">
-        <v>341</v>
+        <v>233</v>
       </c>
       <c r="J19" s="8"/>
       <c r="K19" s="8"/>
@@ -6869,30 +6867,30 @@
       <c r="Z19" s="8"/>
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="B20" s="34" t="s">
+      <c r="A20" s="27" t="s">
         <v>322</v>
       </c>
-      <c r="C20" s="35" t="s">
-        <v>342</v>
-      </c>
-      <c r="D20" s="36" t="s">
-        <v>343</v>
+      <c r="B20" s="27" t="s">
+        <v>234</v>
+      </c>
+      <c r="C20" s="27" t="s">
+        <v>324</v>
+      </c>
+      <c r="D20" s="28" t="s">
+        <v>325</v>
       </c>
       <c r="E20" s="33" t="s">
-        <v>344</v>
+        <v>326</v>
       </c>
       <c r="F20" s="29" t="s">
-        <v>345</v>
-      </c>
-      <c r="G20" s="37" t="s">
-        <v>346</v>
+        <v>327</v>
+      </c>
+      <c r="G20" s="30" t="s">
+        <v>328</v>
       </c>
       <c r="H20" s="31"/>
       <c r="I20" s="20" t="s">
-        <v>347</v>
+        <v>329</v>
       </c>
       <c r="J20" s="8"/>
       <c r="K20" s="8"/>
@@ -6914,29 +6912,29 @@
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="8" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="B21" s="34" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="C21" s="35" t="s">
-        <v>348</v>
-      </c>
-      <c r="D21" s="36" t="s">
-        <v>349</v>
+        <v>331</v>
+      </c>
+      <c r="D21" s="28" t="s">
+        <v>332</v>
       </c>
       <c r="E21" s="33" t="s">
-        <v>350</v>
+        <v>333</v>
       </c>
       <c r="F21" s="29" t="s">
-        <v>351</v>
-      </c>
-      <c r="G21" s="37" t="s">
-        <v>352</v>
+        <v>334</v>
+      </c>
+      <c r="G21" s="30" t="s">
+        <v>335</v>
       </c>
       <c r="H21" s="31"/>
       <c r="I21" s="20" t="s">
-        <v>353</v>
+        <v>336</v>
       </c>
       <c r="J21" s="8"/>
       <c r="K21" s="8"/>
@@ -6958,29 +6956,29 @@
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="8" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="B22" s="34" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="C22" s="35" t="s">
-        <v>354</v>
-      </c>
-      <c r="D22" s="36" t="s">
-        <v>355</v>
+        <v>338</v>
+      </c>
+      <c r="D22" s="28" t="s">
+        <v>339</v>
       </c>
       <c r="E22" s="33" t="s">
-        <v>356</v>
+        <v>340</v>
       </c>
       <c r="F22" s="29" t="s">
-        <v>357</v>
-      </c>
-      <c r="G22" s="38" t="s">
-        <v>358</v>
+        <v>341</v>
+      </c>
+      <c r="G22" s="30" t="s">
+        <v>342</v>
       </c>
       <c r="H22" s="31"/>
       <c r="I22" s="20" t="s">
-        <v>359</v>
+        <v>343</v>
       </c>
       <c r="J22" s="8"/>
       <c r="K22" s="8"/>
@@ -7001,30 +6999,30 @@
       <c r="Z22" s="8"/>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="39" t="s">
-        <v>360</v>
+      <c r="A23" s="8" t="s">
+        <v>73</v>
       </c>
       <c r="B23" s="34" t="s">
-        <v>1</v>
+        <v>344</v>
       </c>
       <c r="C23" s="35" t="s">
-        <v>220</v>
+        <v>345</v>
       </c>
       <c r="D23" s="28" t="s">
-        <v>98</v>
+        <v>346</v>
       </c>
       <c r="E23" s="33" t="s">
-        <v>99</v>
+        <v>347</v>
       </c>
       <c r="F23" s="29" t="s">
-        <v>100</v>
+        <v>348</v>
       </c>
       <c r="G23" s="30" t="s">
-        <v>98</v>
+        <v>346</v>
       </c>
       <c r="H23" s="31"/>
       <c r="I23" s="20" t="s">
-        <v>101</v>
+        <v>349</v>
       </c>
       <c r="J23" s="8"/>
       <c r="K23" s="8"/>
@@ -7044,7 +7042,182 @@
       <c r="Y23" s="8"/>
       <c r="Z23" s="8"/>
     </row>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="B24" s="34" t="s">
+        <v>330</v>
+      </c>
+      <c r="C24" s="35" t="s">
+        <v>350</v>
+      </c>
+      <c r="D24" s="36" t="s">
+        <v>351</v>
+      </c>
+      <c r="E24" s="33" t="s">
+        <v>352</v>
+      </c>
+      <c r="F24" s="29" t="s">
+        <v>353</v>
+      </c>
+      <c r="G24" s="37" t="s">
+        <v>354</v>
+      </c>
+      <c r="H24" s="31"/>
+      <c r="I24" s="20" t="s">
+        <v>355</v>
+      </c>
+      <c r="J24" s="8"/>
+      <c r="K24" s="8"/>
+      <c r="L24" s="8"/>
+      <c r="M24" s="8"/>
+      <c r="N24" s="8"/>
+      <c r="O24" s="8"/>
+      <c r="P24" s="8"/>
+      <c r="Q24" s="8"/>
+      <c r="R24" s="8"/>
+      <c r="S24" s="8"/>
+      <c r="T24" s="8"/>
+      <c r="U24" s="8"/>
+      <c r="V24" s="8"/>
+      <c r="W24" s="8"/>
+      <c r="X24" s="8"/>
+      <c r="Y24" s="8"/>
+      <c r="Z24" s="8"/>
+    </row>
+    <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="B25" s="34" t="s">
+        <v>337</v>
+      </c>
+      <c r="C25" s="35" t="s">
+        <v>356</v>
+      </c>
+      <c r="D25" s="36" t="s">
+        <v>357</v>
+      </c>
+      <c r="E25" s="33" t="s">
+        <v>358</v>
+      </c>
+      <c r="F25" s="29" t="s">
+        <v>359</v>
+      </c>
+      <c r="G25" s="37" t="s">
+        <v>360</v>
+      </c>
+      <c r="H25" s="31"/>
+      <c r="I25" s="20" t="s">
+        <v>361</v>
+      </c>
+      <c r="J25" s="8"/>
+      <c r="K25" s="8"/>
+      <c r="L25" s="8"/>
+      <c r="M25" s="8"/>
+      <c r="N25" s="8"/>
+      <c r="O25" s="8"/>
+      <c r="P25" s="8"/>
+      <c r="Q25" s="8"/>
+      <c r="R25" s="8"/>
+      <c r="S25" s="8"/>
+      <c r="T25" s="8"/>
+      <c r="U25" s="8"/>
+      <c r="V25" s="8"/>
+      <c r="W25" s="8"/>
+      <c r="X25" s="8"/>
+      <c r="Y25" s="8"/>
+      <c r="Z25" s="8"/>
+    </row>
+    <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="B26" s="34" t="s">
+        <v>344</v>
+      </c>
+      <c r="C26" s="35" t="s">
+        <v>362</v>
+      </c>
+      <c r="D26" s="36" t="s">
+        <v>363</v>
+      </c>
+      <c r="E26" s="33" t="s">
+        <v>364</v>
+      </c>
+      <c r="F26" s="29" t="s">
+        <v>365</v>
+      </c>
+      <c r="G26" s="38" t="s">
+        <v>366</v>
+      </c>
+      <c r="H26" s="31"/>
+      <c r="I26" s="20" t="s">
+        <v>367</v>
+      </c>
+      <c r="J26" s="8"/>
+      <c r="K26" s="8"/>
+      <c r="L26" s="8"/>
+      <c r="M26" s="8"/>
+      <c r="N26" s="8"/>
+      <c r="O26" s="8"/>
+      <c r="P26" s="8"/>
+      <c r="Q26" s="8"/>
+      <c r="R26" s="8"/>
+      <c r="S26" s="8"/>
+      <c r="T26" s="8"/>
+      <c r="U26" s="8"/>
+      <c r="V26" s="8"/>
+      <c r="W26" s="8"/>
+      <c r="X26" s="8"/>
+      <c r="Y26" s="8"/>
+      <c r="Z26" s="8"/>
+    </row>
+    <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="39" t="s">
+        <v>368</v>
+      </c>
+      <c r="B27" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="C27" s="35" t="s">
+        <v>220</v>
+      </c>
+      <c r="D27" s="28" t="s">
+        <v>98</v>
+      </c>
+      <c r="E27" s="33" t="s">
+        <v>99</v>
+      </c>
+      <c r="F27" s="29" t="s">
+        <v>100</v>
+      </c>
+      <c r="G27" s="30" t="s">
+        <v>98</v>
+      </c>
+      <c r="H27" s="31"/>
+      <c r="I27" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="J27" s="8"/>
+      <c r="K27" s="8"/>
+      <c r="L27" s="8"/>
+      <c r="M27" s="8"/>
+      <c r="N27" s="8"/>
+      <c r="O27" s="8"/>
+      <c r="P27" s="8"/>
+      <c r="Q27" s="8"/>
+      <c r="R27" s="8"/>
+      <c r="S27" s="8"/>
+      <c r="T27" s="8"/>
+      <c r="U27" s="8"/>
+      <c r="V27" s="8"/>
+      <c r="W27" s="8"/>
+      <c r="X27" s="8"/>
+      <c r="Y27" s="8"/>
+      <c r="Z27" s="8"/>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -7069,32 +7242,32 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.1581632653061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.1377551020408"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.6173469387755"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="5.85204081632653"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.7602040816327"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="35.1887755102041"/>
-    <col collapsed="false" hidden="false" max="14" min="7" style="0" width="7.91836734693878"/>
-    <col collapsed="false" hidden="false" max="25" min="15" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.3163265306122"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.8571428571429"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.20918367346939"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="37.7091836734694"/>
+    <col collapsed="false" hidden="false" max="14" min="7" style="0" width="8.45918367346939"/>
+    <col collapsed="false" hidden="false" max="25" min="15" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="19.0765306122449"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>361</v>
+        <v>369</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>362</v>
+        <v>370</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>363</v>
+        <v>371</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>364</v>
+        <v>372</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>365</v>
+        <v>373</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="8"/>
@@ -7119,20 +7292,20 @@
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="8" t="s">
-        <v>366</v>
+        <v>374</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>367</v>
+        <v>375</v>
       </c>
       <c r="C2" s="40" t="str">
         <f aca="true">TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v>2020-07-21  15-03</v>
+        <v>2020-09-16  18-58</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>368</v>
+        <v>376</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>369</v>
+        <v>377</v>
       </c>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>

</xml_diff>